<commit_message>
New update fo Michael
</commit_message>
<xml_diff>
--- a/EPUI_Data_All.xlsx
+++ b/EPUI_Data_All.xlsx
@@ -65812,8 +65812,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A7E2C7718986FB4B9241671D99B1FB8D" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eb0a6780dfcebf4ad9a2120d556531c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0dab513-4ef6-4f68-a4e8-eada123e36a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e3f36e602dc7511ed11b99db5cb5355" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A7E2C7718986FB4B9241671D99B1FB8D" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bab69e7af17cb87b7da0e754a26d1d22">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0dab513-4ef6-4f68-a4e8-eada123e36a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31224f15db28d4671cd82e2d1f828525" ns2:_="">
     <xsd:import namespace="c0dab513-4ef6-4f68-a4e8-eada123e36a9"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -65827,6 +65827,7 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -65867,6 +65868,11 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -65985,21 +65991,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF67E8A-C4B0-4018-A47E-CF01A17BB828}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c0dab513-4ef6-4f68-a4e8-eada123e36a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F86CF9-D0C8-45EB-AA2B-4CF6AB88A239}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>